<commit_message>
fix excel Result table
</commit_message>
<xml_diff>
--- a/Data/Input/FilteredInvoices.xlsx
+++ b/Data/Input/FilteredInvoices.xlsx
@@ -35,40 +35,40 @@
     <x:t>Invoice Url</x:t>
   </x:si>
   <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bzfw5m88g0fymg6lk5cle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/12.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>agkf70jn9satt1rxtvyy6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/8.jpg</x:t>
+  </x:si>
+  <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>n4zdfr8rz4cdlxzf49uy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08-07-2024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/12.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>j6qky8ysjflms7kciqj97i</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14-07-2024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/8.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>g15db3dv9zupp579hzbzm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15-07-2024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/7.jpg</x:t>
+    <x:t>wj34k48z92mgkik0lpdt1g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/10.jpg</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
fix download (add Overwrite to the Move File)
</commit_message>
<xml_diff>
--- a/Data/Input/FilteredInvoices.xlsx
+++ b/Data/Input/FilteredInvoices.xlsx
@@ -38,37 +38,70 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>bzfw5m88g0fymg6lk5cle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16-07-2024</x:t>
+    <x:t>gw2odrctzelzpzjf3mmslp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28-07-2024</x:t>
   </x:si>
   <x:si>
     <x:t>https://rpachallengeocr.azurewebsites.net/invoices/12.jpg</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>agkf70jn9satt1rxtvyy6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>07-07-2024</x:t>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>538o6gypasvtnt0sfq1ivr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>06-08-2024</x:t>
   </x:si>
   <x:si>
     <x:t>https://rpachallengeocr.azurewebsites.net/invoices/8.jpg</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>wj34k48z92mgkik0lpdt1g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25-07-2024</x:t>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>zs2l4nrxtyprw8hh31dpdq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-07-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/7.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ste1r42xtv20yf084aj2t</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20-08-2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rpachallengeocr.azurewebsites.net/invoices/11.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>snspz98nxw80ux68n4q69n</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10-07-2024</x:t>
   </x:si>
   <x:si>
     <x:t>https://rpachallengeocr.azurewebsites.net/invoices/10.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>y0yvyji9lgkln1b210be98</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19-07-2024</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -476,6 +509,48 @@
         <x:v>15</x:v>
       </x:c>
     </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>